<commit_message>
campus image /shiny update
</commit_message>
<xml_diff>
--- a/inst/geog178_gradebook_2020/data/grades.xlsx
+++ b/inst/geog178_gradebook_2020/data/grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikejohnson/Documents/GitHub/geog178_2020/inst/geog178_gradebook_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7570ED3B-92F4-7A47-A812-00B03649ECFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB8CA21-36C6-FF46-A888-9D27A6EF6F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lab1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="201">
   <si>
     <t>9514696</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t>I was looking for the nested minimumn between all combinations of points</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Great! Just missing the descriptsion of for loops and if statements</t>
@@ -1087,7 +1084,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K43" sqref="K43"/>
+      <selection pane="topRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,13 +1149,13 @@
         <v>54</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1197,7 +1194,7 @@
         <v>18</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1232,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>SUM(C4:J4)</f>
+        <f t="shared" ref="K4:K18" si="0">SUM(C4:J4)</f>
         <v>9</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1271,11 +1268,11 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f>SUM(C5:J5)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1310,11 +1307,11 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f>SUM(C6:J6)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1349,11 +1346,11 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1388,11 +1385,11 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1427,11 +1424,11 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1466,11 +1463,11 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1505,11 +1502,11 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>SUM(C11:J11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1544,11 +1541,11 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1583,11 +1580,11 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1622,11 +1619,11 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1661,11 +1658,11 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <f>SUM(C15:J15)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1700,11 +1697,11 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <f>SUM(C16:J16)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1739,11 +1736,11 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <f>SUM(C17:J17)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1778,11 +1775,11 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f>SUM(C18:J18)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1795,7 +1792,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1830,11 +1827,11 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <f>SUM(C20:J20)</f>
+        <f t="shared" ref="K20:K29" si="1">SUM(C20:J20)</f>
         <v>8</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1869,11 +1866,11 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <f>SUM(C21:J21)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1908,11 +1905,11 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <f>SUM(C22:J22)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1947,11 +1944,11 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <f>SUM(C23:J23)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1986,11 +1983,11 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f>SUM(C24:J24)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2025,11 +2022,11 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <f>SUM(C25:J25)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2064,11 +2061,11 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <f>SUM(C26:J26)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2103,11 +2100,11 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <f>SUM(C27:J27)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2142,11 +2139,11 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <f>SUM(C28:J28)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2181,58 +2178,58 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f>SUM(C29:J29)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30" s="13">
         <f>AVERAGE(C3:C29)</f>
         <v>0.92</v>
       </c>
       <c r="D30" s="13">
-        <f t="shared" ref="D30:K30" si="0">AVERAGE(D3:D29)</f>
+        <f t="shared" ref="D30:K30" si="2">AVERAGE(D3:D29)</f>
         <v>0.92</v>
       </c>
       <c r="E30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.76</v>
       </c>
       <c r="J30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2267,7 +2264,7 @@
     <col min="10" max="10" width="12.1640625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="213.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2308,13 +2305,13 @@
         <v>54</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2357,7 +2354,7 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -2395,11 +2392,11 @@
         <v>1</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L3:L29" si="0">SUM(C4:K4)</f>
+        <f t="shared" ref="L4:L29" si="0">SUM(C4:K4)</f>
         <v>10</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2441,7 +2438,7 @@
         <v>3.5</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2483,7 +2480,7 @@
         <v>10</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2495,7 +2492,7 @@
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2537,7 +2534,7 @@
         <v>7.5</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -2579,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -2621,7 +2618,7 @@
         <v>10</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -2663,7 +2660,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -2705,7 +2702,7 @@
         <v>10</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -2747,7 +2744,7 @@
         <v>10</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2789,7 +2786,7 @@
         <v>9.5</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -2802,7 +2799,7 @@
       <c r="G15" s="3"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -2844,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -2886,7 +2883,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2928,7 +2925,7 @@
         <v>8</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -2940,7 +2937,7 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -2982,7 +2979,7 @@
         <v>10</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -3024,7 +3021,7 @@
         <v>10</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -3036,7 +3033,7 @@
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -3078,7 +3075,7 @@
         <v>8</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -3120,7 +3117,7 @@
         <v>8</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -3162,7 +3159,7 @@
         <v>9.75</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -3204,7 +3201,7 @@
         <v>9.5</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -3246,7 +3243,7 @@
         <v>10</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -3288,7 +3285,7 @@
         <v>10</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -3330,15 +3327,15 @@
         <v>10</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C3:C29)</f>
@@ -3381,7 +3378,7 @@
         <v>8.5340909090909083</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3415,6 +3412,7 @@
     <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="201.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -3425,22 +3423,22 @@
         <v>56</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>69</v>
@@ -3455,13 +3453,13 @@
         <v>54</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -3505,7 +3503,7 @@
       <c r="C3" s="3"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3543,11 +3541,11 @@
         <v>1</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L3:L29" si="0">SUM(C4:K4)</f>
+        <f t="shared" ref="L4:L18" si="0">SUM(C4:K4)</f>
         <v>7</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3589,7 +3587,7 @@
         <v>6</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -3631,7 +3629,7 @@
         <v>10</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3673,7 +3671,7 @@
         <v>10</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3715,7 +3713,7 @@
         <v>10</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3757,7 +3755,7 @@
         <v>10</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3799,7 +3797,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3841,7 +3839,7 @@
         <v>9</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3883,7 +3881,7 @@
         <v>7</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3925,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3967,7 +3965,7 @@
         <v>10</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3981,7 +3979,7 @@
       <c r="H15" s="3"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3996,7 +3994,7 @@
       <c r="H16" s="3"/>
       <c r="L16" s="2"/>
       <c r="M16" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -4038,7 +4036,7 @@
         <v>10</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -4080,7 +4078,7 @@
         <v>6</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -4093,7 +4091,7 @@
       <c r="C19" s="3"/>
       <c r="L19" s="2"/>
       <c r="M19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -4135,7 +4133,7 @@
         <v>8</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -4177,7 +4175,7 @@
         <v>10</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4190,7 +4188,7 @@
       <c r="C22" s="3"/>
       <c r="L22" s="2"/>
       <c r="M22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4232,7 +4230,7 @@
         <v>8</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4274,7 +4272,7 @@
         <v>10</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4316,7 +4314,7 @@
         <v>10</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -4358,7 +4356,7 @@
         <v>8</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -4400,7 +4398,7 @@
         <v>9</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4442,7 +4440,7 @@
         <v>10</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4484,15 +4482,15 @@
         <v>9</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C3:C29)</f>
@@ -4535,7 +4533,7 @@
         <v>8.9090909090909083</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4551,9 +4549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4823B62A-7463-F44B-8C75-D917A0CEFA5B}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L37" sqref="L37"/>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4572,7 +4570,7 @@
     <col min="12" max="12" width="133.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
@@ -4592,13 +4590,13 @@
         <v>73</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>61</v>
@@ -4607,13 +4605,13 @@
         <v>54</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -4684,11 +4682,11 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>SUM(C4:J4)</f>
+        <f t="shared" ref="K4:K14" si="0">SUM(C4:J4)</f>
         <v>9</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -4723,11 +4721,11 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f>SUM(C5:J5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4762,11 +4760,11 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f>SUM(C6:J6)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -4801,11 +4799,11 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -4840,11 +4838,11 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4879,11 +4877,11 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -4918,11 +4916,11 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -4957,11 +4955,11 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>SUM(C11:J11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -4996,11 +4994,11 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -5035,11 +5033,11 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -5074,11 +5072,11 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -5089,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -5128,7 +5126,7 @@
         <v>10</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -5167,7 +5165,7 @@
         <v>10</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -5202,11 +5200,11 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:K29" si="0">SUM(C18:J18)</f>
+        <f t="shared" ref="K18:K29" si="1">SUM(C18:J18)</f>
         <v>9</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -5217,7 +5215,7 @@
         <v>6</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -5252,11 +5250,11 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -5291,11 +5289,11 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -5306,7 +5304,7 @@
         <v>25</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -5317,7 +5315,7 @@
         <v>15</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -5352,11 +5350,11 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -5391,11 +5389,11 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -5430,11 +5428,11 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -5469,11 +5467,11 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -5508,11 +5506,11 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -5547,55 +5545,58 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C3:C29)</f>
         <v>0.59090909090909094</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:K30" si="1">AVERAGE(D3:D29)</f>
+        <f t="shared" ref="D30:K30" si="2">AVERAGE(D3:D29)</f>
         <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9090909090909092</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7272727272727273</v>
       </c>
       <c r="J30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95454545454545459</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1818181818181817</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -5611,8 +5612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7A4C5C-0F82-F24B-92C2-E56DD2F453FA}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="N11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5641,7 +5642,7 @@
         <v>82</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>75</v>
@@ -5671,13 +5672,13 @@
         <v>54</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -5764,7 +5765,7 @@
         <v>9.5</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -5809,7 +5810,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -5854,7 +5855,7 @@
         <v>10</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -5899,7 +5900,7 @@
         <v>10</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -5944,7 +5945,7 @@
         <v>8</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -5989,7 +5990,7 @@
         <v>10</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -6034,7 +6035,7 @@
         <v>9</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -6079,7 +6080,7 @@
         <v>9</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -6124,7 +6125,7 @@
         <v>8</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -6169,7 +6170,7 @@
         <v>10</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -6214,7 +6215,7 @@
         <v>10</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -6277,7 +6278,7 @@
         <v>10</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -6322,7 +6323,7 @@
         <v>10</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -6367,7 +6368,7 @@
         <v>3</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -6412,7 +6413,7 @@
         <v>4.75</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -6457,7 +6458,7 @@
         <v>10</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -6502,7 +6503,7 @@
         <v>10</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -6547,7 +6548,7 @@
         <v>10</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -6592,7 +6593,7 @@
         <v>10</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -6637,7 +6638,7 @@
         <v>10</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -6682,7 +6683,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -6727,7 +6728,7 @@
         <v>8</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -6772,7 +6773,7 @@
         <v>9</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -6816,7 +6817,7 @@
         <v>10</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -6861,15 +6862,15 @@
         <v>10</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <f>AVERAGE(C3:C29)</f>
@@ -6914,6 +6915,9 @@
       <c r="M30">
         <f t="shared" si="2"/>
         <v>8.57</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -6975,13 +6979,13 @@
         <v>54</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -7014,7 +7018,7 @@
         <v>18</v>
       </c>
       <c r="I3">
-        <f>SUM(C3:G3)</f>
+        <f t="shared" ref="I3:I29" si="0">SUM(C3:G3)</f>
         <v>0</v>
       </c>
     </row>
@@ -7026,7 +7030,7 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <f>SUM(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7038,7 +7042,7 @@
         <v>8</v>
       </c>
       <c r="I5">
-        <f>SUM(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7050,7 +7054,7 @@
         <v>13</v>
       </c>
       <c r="I6">
-        <f>SUM(C6:G6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7062,7 +7066,7 @@
         <v>17</v>
       </c>
       <c r="I7">
-        <f>SUM(C7:G7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7074,7 +7078,7 @@
         <v>19</v>
       </c>
       <c r="I8">
-        <f>SUM(C8:G8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7086,7 +7090,7 @@
         <v>9</v>
       </c>
       <c r="I9">
-        <f>SUM(C9:G9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7098,7 +7102,7 @@
         <v>12</v>
       </c>
       <c r="I10">
-        <f>SUM(C10:G10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7110,7 +7114,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <f>SUM(C11:G11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7122,7 +7126,7 @@
         <v>14</v>
       </c>
       <c r="I12">
-        <f>SUM(C12:G12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7134,7 +7138,7 @@
         <v>11</v>
       </c>
       <c r="I13">
-        <f>SUM(C13:G13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7146,7 +7150,7 @@
         <v>21</v>
       </c>
       <c r="I14">
-        <f>SUM(C14:G14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7158,7 +7162,7 @@
         <v>3</v>
       </c>
       <c r="I15">
-        <f>SUM(C15:G15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7170,7 +7174,7 @@
         <v>7</v>
       </c>
       <c r="I16">
-        <f>SUM(C16:G16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7182,7 +7186,7 @@
         <v>2</v>
       </c>
       <c r="I17">
-        <f>SUM(C17:G17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7194,7 +7198,7 @@
         <v>20</v>
       </c>
       <c r="I18">
-        <f>SUM(C18:G18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7206,7 +7210,7 @@
         <v>6</v>
       </c>
       <c r="I19">
-        <f>SUM(C19:G19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7218,7 +7222,7 @@
         <v>4</v>
       </c>
       <c r="I20">
-        <f>SUM(C20:G20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7230,7 +7234,7 @@
         <v>5</v>
       </c>
       <c r="I21">
-        <f>SUM(C21:G21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7242,7 +7246,7 @@
         <v>25</v>
       </c>
       <c r="I22">
-        <f>SUM(C22:G22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7254,7 +7258,7 @@
         <v>15</v>
       </c>
       <c r="I23">
-        <f>SUM(C23:G23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7266,7 +7270,7 @@
         <v>16</v>
       </c>
       <c r="I24">
-        <f>SUM(C24:G24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7278,7 +7282,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <f>SUM(C25:G25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7290,7 +7294,7 @@
         <v>24</v>
       </c>
       <c r="I26">
-        <f>SUM(C26:G26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7302,7 +7306,7 @@
         <v>23</v>
       </c>
       <c r="I27">
-        <f>SUM(C27:G27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7314,7 +7318,7 @@
         <v>22</v>
       </c>
       <c r="I28">
-        <f>SUM(C28:G28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7326,16 +7330,16 @@
         <v>26</v>
       </c>
       <c r="I29">
-        <f>SUM(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -7352,7 +7356,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7369,31 +7373,31 @@
         <v>56</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -7542,7 +7546,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="13">
-        <f t="shared" ref="I4:I29" si="0">AVERAGE(C6:H6)</f>
+        <f t="shared" ref="I6:I29" si="0">AVERAGE(C6:H6)</f>
         <v>10</v>
       </c>
     </row>
@@ -8284,10 +8288,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <f>'lab1'!K30</f>

</xml_diff>